<commit_message>
Updated with needed test cases for Game 2 and fixed button hover
</commit_message>
<xml_diff>
--- a/Documentation/GameTestCases.xlsx
+++ b/Documentation/GameTestCases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\source\repos\Kanrail\5153-Ethics_Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F69B76-AA75-4711-B491-DCF16DE272E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="1935" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>Feature</t>
   </si>
@@ -144,12 +145,57 @@
   </si>
   <si>
     <t>Out of Bounds Game Over</t>
+  </si>
+  <si>
+    <t>Displays correctly after game loss</t>
+  </si>
+  <si>
+    <t>Game Over Screen</t>
+  </si>
+  <si>
+    <t>GO Restart Button Hover</t>
+  </si>
+  <si>
+    <t>GO Restart Button Press</t>
+  </si>
+  <si>
+    <t>GO Main Menu Button Hover</t>
+  </si>
+  <si>
+    <t>GO Main Menu Button Press</t>
+  </si>
+  <si>
+    <t>Darkens to a slight grey on mouse hover</t>
+  </si>
+  <si>
+    <t>Darkens to almost black and then Redirects player to main menu</t>
+  </si>
+  <si>
+    <t>Darkens to almost black and then restarts the snake game from beginning</t>
+  </si>
+  <si>
+    <t>Game Win</t>
+  </si>
+  <si>
+    <t>Game correctly ends and proceeds to next scene upon reaching 0 pellets</t>
+  </si>
+  <si>
+    <t>Food Pellets Disappear When Eaten</t>
+  </si>
+  <si>
+    <t>Food pellets disappear when eaten by snake</t>
+  </si>
+  <si>
+    <t>Snake Increases in Size</t>
+  </si>
+  <si>
+    <t>Snake increases in size when pellet eaten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,17 +540,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -747,35 +793,99 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="E24" t="s">
-        <v>10</v>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -784,12 +894,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1016,15 +1123,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
+    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1049,18 +1168,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
-    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated and combined the test case document
</commit_message>
<xml_diff>
--- a/Documentation/GameTestCases.xlsx
+++ b/Documentation/GameTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\source\repos\Kanrail\5153-Ethics_Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F69B76-AA75-4711-B491-DCF16DE272E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97589150-867D-4E5B-8B46-31F3C31EE5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
   <si>
     <t>Feature</t>
   </si>
@@ -190,19 +190,94 @@
   </si>
   <si>
     <t>Snake increases in size when pellet eaten</t>
+  </si>
+  <si>
+    <t>ball starts moving</t>
+  </si>
+  <si>
+    <t>right bar moves up</t>
+  </si>
+  <si>
+    <t>right bar moves down</t>
+  </si>
+  <si>
+    <t>w key</t>
+  </si>
+  <si>
+    <t>left bar moves up</t>
+  </si>
+  <si>
+    <t>s key</t>
+  </si>
+  <si>
+    <t>left bar moves down</t>
+  </si>
+  <si>
+    <t>ball moves in opposite direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displays game over with winner player </t>
+  </si>
+  <si>
+    <t>Main Menu Button Hover</t>
+  </si>
+  <si>
+    <t>Main Menu Button Press</t>
+  </si>
+  <si>
+    <t>highlights grey on mouse hold and redirects player to main menu</t>
+  </si>
+  <si>
+    <t>Player waits 2.5 seconds</t>
+  </si>
+  <si>
+    <t>Up arrow key</t>
+  </si>
+  <si>
+    <t>Down arrow key</t>
+  </si>
+  <si>
+    <t>Ball hits on bar</t>
+  </si>
+  <si>
+    <t>Ball miss to hit on bar</t>
+  </si>
+  <si>
+    <t>Game Rematch Screen</t>
+  </si>
+  <si>
+    <t>game transitions to rematch screen after game loss</t>
+  </si>
+  <si>
+    <t>Rematch Button Hover</t>
+  </si>
+  <si>
+    <t>Rematch Button Press</t>
+  </si>
+  <si>
+    <t>Game restarts</t>
+  </si>
+  <si>
+    <t>Pong Game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,8 +300,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +747,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -798,6 +874,9 @@
       <c r="D22" t="s">
         <v>52</v>
       </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -806,6 +885,9 @@
       <c r="D23" t="s">
         <v>54</v>
       </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
@@ -847,6 +929,9 @@
       <c r="D27" t="s">
         <v>50</v>
       </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
@@ -855,6 +940,9 @@
       <c r="D28" t="s">
         <v>40</v>
       </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
@@ -863,6 +951,9 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
@@ -871,6 +962,9 @@
       <c r="D30" t="s">
         <v>48</v>
       </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
@@ -879,6 +973,9 @@
       <c r="D31" t="s">
         <v>46</v>
       </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
@@ -886,6 +983,147 @@
       </c>
       <c r="D32" t="s">
         <v>47</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -894,12 +1132,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002F3B64CF3F87534C89394D192F37FE03" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc92f62612f157ce92826da6fac2f568">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1a853a03-70b7-4e88-b9d6-862a6d0d513b" xmlns:ns4="006257e6-8004-434d-9d5c-8648ed86a46d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53f9340ff9bd35e08117073a0c9a3ff6" ns3:_="" ns4:_="">
     <xsd:import namespace="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
@@ -1122,7 +1354,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1131,24 +1363,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
-    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E9AF1B-1443-4248-BC04-1FB939548151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1167,10 +1388,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
+    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Just in case the beginning of the ethics question decides to delete itself, going to do periodic commits to make sure nothing is lost
</commit_message>
<xml_diff>
--- a/Documentation/GameTestCases.xlsx
+++ b/Documentation/GameTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\source\repos\Kanrail\5153-Ethics_Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97589150-867D-4E5B-8B46-31F3C31EE5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55859DA8-942B-4D01-A05A-D36CCA337204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
   <si>
     <t>Feature</t>
   </si>
@@ -117,36 +117,6 @@
     <t>Snake MG</t>
   </si>
   <si>
-    <t>Snake changes direction from user input</t>
-  </si>
-  <si>
-    <t>Snake Moves</t>
-  </si>
-  <si>
-    <t>Food Pellets Appear</t>
-  </si>
-  <si>
-    <t>Food pellets appear randomly around the play area</t>
-  </si>
-  <si>
-    <t>Game ends if snake collides with boundaries</t>
-  </si>
-  <si>
-    <t>Snake Collision Game Over</t>
-  </si>
-  <si>
-    <t>Game ends if snake collides with itself</t>
-  </si>
-  <si>
-    <t>Score Counter</t>
-  </si>
-  <si>
-    <t>Score counter updates and accurately displays remaining pellets needed</t>
-  </si>
-  <si>
-    <t>Out of Bounds Game Over</t>
-  </si>
-  <si>
     <t>Displays correctly after game loss</t>
   </si>
   <si>
@@ -174,24 +144,9 @@
     <t>Darkens to almost black and then restarts the snake game from beginning</t>
   </si>
   <si>
-    <t>Game Win</t>
-  </si>
-  <si>
     <t>Game correctly ends and proceeds to next scene upon reaching 0 pellets</t>
   </si>
   <si>
-    <t>Food Pellets Disappear When Eaten</t>
-  </si>
-  <si>
-    <t>Food pellets disappear when eaten by snake</t>
-  </si>
-  <si>
-    <t>Snake Increases in Size</t>
-  </si>
-  <si>
-    <t>Snake increases in size when pellet eaten</t>
-  </si>
-  <si>
     <t>ball starts moving</t>
   </si>
   <si>
@@ -201,64 +156,187 @@
     <t>right bar moves down</t>
   </si>
   <si>
-    <t>w key</t>
-  </si>
-  <si>
     <t>left bar moves up</t>
   </si>
   <si>
-    <t>s key</t>
-  </si>
-  <si>
     <t>left bar moves down</t>
   </si>
   <si>
-    <t>ball moves in opposite direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">displays game over with winner player </t>
-  </si>
-  <si>
-    <t>Main Menu Button Hover</t>
-  </si>
-  <si>
-    <t>Main Menu Button Press</t>
-  </si>
-  <si>
-    <t>highlights grey on mouse hold and redirects player to main menu</t>
-  </si>
-  <si>
-    <t>Player waits 2.5 seconds</t>
-  </si>
-  <si>
-    <t>Up arrow key</t>
-  </si>
-  <si>
-    <t>Down arrow key</t>
-  </si>
-  <si>
-    <t>Ball hits on bar</t>
-  </si>
-  <si>
-    <t>Ball miss to hit on bar</t>
-  </si>
-  <si>
-    <t>Game Rematch Screen</t>
-  </si>
-  <si>
-    <t>game transitions to rematch screen after game loss</t>
-  </si>
-  <si>
-    <t>Rematch Button Hover</t>
-  </si>
-  <si>
-    <t>Rematch Button Press</t>
-  </si>
-  <si>
-    <t>Game restarts</t>
-  </si>
-  <si>
     <t>Pong Game</t>
+  </si>
+  <si>
+    <t>Scene Start: Pellet Spawn</t>
+  </si>
+  <si>
+    <t>Scene Start: Snake Starts Moving</t>
+  </si>
+  <si>
+    <t>Single pellet starts on screen and food pellets start randomly appearing within the white boundaries</t>
+  </si>
+  <si>
+    <t>Snake starts moving to right</t>
+  </si>
+  <si>
+    <t>Snake Collision: Food Pellet</t>
+  </si>
+  <si>
+    <t>Snake Collision: Top Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Bottom Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Left Border</t>
+  </si>
+  <si>
+    <t>Snake Collision: Right Border</t>
+  </si>
+  <si>
+    <t>Game shifts to game over screen</t>
+  </si>
+  <si>
+    <t>Snake Collision: Tail</t>
+  </si>
+  <si>
+    <t>Food pellet disappears, snake grows by one tail piece, score counter decreased by 1</t>
+  </si>
+  <si>
+    <t>Snake Movement: Up key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Down key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Left key pressed</t>
+  </si>
+  <si>
+    <t>Snake Movement: Right key pressed</t>
+  </si>
+  <si>
+    <t>Snake starts moving down, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving right, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving left, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Snake starts moving up, tail follows at pivot point</t>
+  </si>
+  <si>
+    <t>Score counter initializes to 10 (default for now)</t>
+  </si>
+  <si>
+    <t>Scene Start: Score Counter Initializes</t>
+  </si>
+  <si>
+    <t>Score Counter Updated</t>
+  </si>
+  <si>
+    <t>Accurately displays remaining pellets needed</t>
+  </si>
+  <si>
+    <t>Score counter reaches 0</t>
+  </si>
+  <si>
+    <t>Start game button hover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End game button hover </t>
+  </si>
+  <si>
+    <t>Start game button press</t>
+  </si>
+  <si>
+    <t>switch to pong game scene</t>
+  </si>
+  <si>
+    <t>End game button press</t>
+  </si>
+  <si>
+    <t>switch to main menu</t>
+  </si>
+  <si>
+    <t>Scene starts player waits 2.5 seconds</t>
+  </si>
+  <si>
+    <t>Press up arrow key</t>
+  </si>
+  <si>
+    <t>Press down arrow key</t>
+  </si>
+  <si>
+    <t>Press w key</t>
+  </si>
+  <si>
+    <t>Press s key</t>
+  </si>
+  <si>
+    <t>Ball hits on top border</t>
+  </si>
+  <si>
+    <t>ball bounces down at an angle same direction in which it hit</t>
+  </si>
+  <si>
+    <t>Ball hits on bottom border</t>
+  </si>
+  <si>
+    <t>ball bounces up at an angle same direction in which it hit</t>
+  </si>
+  <si>
+    <t>Ball hits on left bar</t>
+  </si>
+  <si>
+    <t>ball moves in opposite direction randomly</t>
+  </si>
+  <si>
+    <t>Ball hits on right bar</t>
+  </si>
+  <si>
+    <t>Ball miss to hit on right bar</t>
+  </si>
+  <si>
+    <t>displays game over with which player wins</t>
+  </si>
+  <si>
+    <t>Ball miss to hit on left bar</t>
+  </si>
+  <si>
+    <t>Player 1 win screen</t>
+  </si>
+  <si>
+    <t>screen displays if player1 wins</t>
+  </si>
+  <si>
+    <t>Player 2 win screen</t>
+  </si>
+  <si>
+    <t>screen displays if player2 wins</t>
+  </si>
+  <si>
+    <t>Player 1 screen rematch button hover</t>
+  </si>
+  <si>
+    <t>Player 1 screen menu button hover</t>
+  </si>
+  <si>
+    <t>Player 2 screen rematch button hover</t>
+  </si>
+  <si>
+    <t>Player 2 screen menu button hover</t>
+  </si>
+  <si>
+    <t>Player 1 screen rematch button press</t>
+  </si>
+  <si>
+    <t>switch to the game scene</t>
+  </si>
+  <si>
+    <t>Player 1 screen menu button press</t>
+  </si>
+  <si>
+    <t>Player 2 screen rematch button press</t>
   </si>
 </sst>
 </file>
@@ -300,9 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,7 +444,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -415,7 +496,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -617,10 +698,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +831,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -839,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -847,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -858,10 +942,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -869,21 +953,21 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -891,10 +975,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -902,10 +986,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -913,10 +997,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -924,10 +1008,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -935,10 +1019,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -946,10 +1030,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -957,10 +1041,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -968,10 +1052,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -979,27 +1063,32 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1007,10 +1096,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1018,10 +1107,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1029,10 +1118,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1040,10 +1129,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1051,32 +1140,27 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
         <v>71</v>
       </c>
-      <c r="D40" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>72</v>
-      </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1084,10 +1168,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1095,10 +1179,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1106,32 +1190,270 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002F3B64CF3F87534C89394D192F37FE03" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc92f62612f157ce92826da6fac2f568">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1a853a03-70b7-4e88-b9d6-862a6d0d513b" xmlns:ns4="006257e6-8004-434d-9d5c-8648ed86a46d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53f9340ff9bd35e08117073a0c9a3ff6" ns3:_="" ns4:_="">
     <xsd:import namespace="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
@@ -1354,22 +1676,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
+    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E9AF1B-1443-4248-BC04-1FB939548151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1386,29 +1718,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8A67A2-5DDB-4C40-88B1-8FE14C708844}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76F575D-EE7F-4E8F-A345-86B9CCF1C624}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="006257e6-8004-434d-9d5c-8648ed86a46d"/>
-    <ds:schemaRef ds:uri="1a853a03-70b7-4e88-b9d6-862a6d0d513b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>